<commit_message>
Changed domain name from lvasc to bri for belt and road initiative, fixed bug where light verb 'give' had a catvar alternate of 'gift' which caused out of range belief strengths because it was doubling up on the strength from gift in the triggers and give in the light verbs, and added some items to bri lexicons
</commit_message>
<xml_diff>
--- a/ARLIS_contents.xlsx
+++ b/ARLIS_contents.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Lexical item</t>
   </si>
@@ -35,13 +35,22 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>bribe</t>
+  </si>
+  <si>
+    <t>//Might need to check the -1 sentiment with positive belief category... it's interestiing</t>
+  </si>
+  <si>
+    <t>money</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -51,6 +60,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -66,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -74,6 +84,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -369,6 +382,42 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-1.0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-1.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated detection app to handle domain name in other functions, added ability to do experimentation of stance detection by showing all predicate argument pairs, updated BRI lexicons
</commit_message>
<xml_diff>
--- a/ARLIS_contents.xlsx
+++ b/ARLIS_contents.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>Lexical item</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Sentiment Value</t>
   </si>
   <si>
+    <t>Added just to get examples out</t>
+  </si>
+  <si>
     <t>economy</t>
   </si>
   <si>
@@ -40,10 +43,16 @@
     <t>bribe</t>
   </si>
   <si>
-    <t>//Might need to check the -1 sentiment with positive belief category... it's interestiing</t>
-  </si>
-  <si>
     <t>money</t>
+  </si>
+  <si>
+    <t>sovereignty</t>
+  </si>
+  <si>
+    <t>slavery</t>
+  </si>
+  <si>
+    <t>project</t>
   </si>
 </sst>
 </file>
@@ -315,85 +324,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>-1.0</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>-1.0</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
         <v>-1.0</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-1.0</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -401,10 +431,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -412,10 +445,83 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
         <v>-1.0</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-1.0</v>
+      </c>
+      <c r="D11" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-1.0</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-1.0</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added economic to BRI content lexicon
</commit_message>
<xml_diff>
--- a/ARLIS_contents.xlsx
+++ b/ARLIS_contents.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Lexical item</t>
   </si>
@@ -52,7 +52,13 @@
     <t>slavery</t>
   </si>
   <si>
+    <t>RESTRICT</t>
+  </si>
+  <si>
     <t>project</t>
+  </si>
+  <si>
+    <t>economic</t>
   </si>
 </sst>
 </file>
@@ -486,8 +492,8 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="2">
         <v>-1.0</v>
@@ -498,7 +504,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
@@ -512,7 +518,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>6</v>
@@ -521,6 +527,34 @@
         <v>1.0</v>
       </c>
       <c r="D15" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-1.0</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-1.0</v>
+      </c>
+      <c r="D17" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added resources to contents lexicon
</commit_message>
<xml_diff>
--- a/ARLIS_contents.xlsx
+++ b/ARLIS_contents.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodieslab/docker_build/ask_detection/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3343F7FC-66D3-8046-B559-12435AB43FA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>Lexical item</t>
   </si>
@@ -59,65 +68,78 @@
   </si>
   <si>
     <t>economic</t>
+  </si>
+  <si>
+    <t>impediment</t>
+  </si>
+  <si>
+    <t>resources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -307,20 +329,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -334,7 +361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -342,13 +369,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -356,13 +383,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -370,13 +397,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -384,13 +411,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -398,13 +425,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -412,13 +439,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -426,13 +453,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -440,13 +467,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -454,13 +481,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -468,13 +495,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D11" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -482,13 +509,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -496,13 +523,13 @@
         <v>13</v>
       </c>
       <c r="C13" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -510,13 +537,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -524,13 +551,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -538,13 +565,13 @@
         <v>5</v>
       </c>
       <c r="C16" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -552,13 +579,55 @@
         <v>6</v>
       </c>
       <c r="C17" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D20" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added get to light verbs list, added isis domain, and updated allen sentiment to use latest model
</commit_message>
<xml_diff>
--- a/ARLIS_contents.xlsx
+++ b/ARLIS_contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodieslab/docker_build/ask_detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3343F7FC-66D3-8046-B559-12435AB43FA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E953210-49FD-F84B-A0B7-6B8E734FAD63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>Lexical item</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>economic</t>
-  </si>
-  <si>
-    <t>impediment</t>
   </si>
   <si>
     <t>resources</t>
@@ -339,10 +336,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -589,7 +586,7 @@
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="2">
@@ -601,33 +598,20 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="2">
         <v>-1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2">
-        <v>-1</v>
-      </c>
-      <c r="D20" s="2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>